<commit_message>
bug fix in ggplot_resp_cat_vf - had non-categorical measure variable in it
</commit_message>
<xml_diff>
--- a/Data/Delphi round 1/response sheets/Jim Sm-Wr - give your expert opinion on woodland condition111.xlsx
+++ b/Data/Delphi round 1/response sheets/Jim Sm-Wr - give your expert opinion on woodland condition111.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Delphi round 1/response sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Woodland-condition/Data/Delphi round 1/response sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="736" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{910B1343-EFFD-48BC-BD43-1C0B7A111E48}"/>
+  <xr:revisionPtr revIDLastSave="762" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3831EB0A-3C82-4150-BC89-FD13235F2835}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4815" windowWidth="16440" windowHeight="28320" tabRatio="712" firstSheet="12" activeTab="14" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="712" activeTab="3" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree age distribution" sheetId="20" r:id="rId1"/>
@@ -838,7 +838,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -966,6 +966,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1081,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1126,6 +1134,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4435,12 +4444,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -4453,15 +4465,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
@@ -4880,7 +4895,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
-          <c:min val="0"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5208,20 +5223,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'N tree &amp; shrub spp.'!$A$10:$A$17</c:f>
+              <c:f>'N tree &amp; shrub spp.'!$A$10:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
@@ -5229,20 +5262,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'N tree &amp; shrub spp.'!$B$10:$B$17</c:f>
+              <c:f>'N tree &amp; shrub spp.'!$B$10:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -18669,8 +18720,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{34E56704-5D90-4D5C-AC12-5904D85A5240}" name="Table156" displayName="Table156" ref="A9:B17" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A9:B17" xr:uid="{AB04B7AD-16D4-48B1-9771-A4B9EAE35B9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{34E56704-5D90-4D5C-AC12-5904D85A5240}" name="Table156" displayName="Table156" ref="A9:B19" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A9:B19" xr:uid="{AB04B7AD-16D4-48B1-9771-A4B9EAE35B9B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:B17">
     <sortCondition ref="A9:A17"/>
   </sortState>
@@ -22229,10 +22280,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3248C487-FA81-4908-B7DC-7E550BAD9141}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" activeCellId="1" sqref="B46 J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22429,7 +22480,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>164</v>
       </c>
@@ -22445,7 +22496,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>166</v>
       </c>
@@ -22461,7 +22512,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>130</v>
       </c>
@@ -22477,7 +22528,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>94</v>
       </c>
@@ -22493,7 +22544,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>151</v>
       </c>
@@ -22509,7 +22560,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>150</v>
       </c>
@@ -22524,6 +22575,12 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="30"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="30"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:H8" xr:uid="{3248C487-FA81-4908-B7DC-7E550BAD9141}">
@@ -22542,7 +22599,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22624,7 +22681,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>9</v>
@@ -22646,10 +22703,10 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -22669,10 +22726,10 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2">
         <v>75</v>
-      </c>
-      <c r="B12" s="2">
-        <v>95</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -22683,15 +22740,19 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2">
+        <v>100</v>
+      </c>
+      <c r="B14" s="2">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -22964,7 +23025,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23486,8 +23547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E3BDB2-4936-4583-A0D1-731A826C7FE6}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23588,10 +23649,10 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -23611,10 +23672,10 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B12" s="2">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -23625,15 +23686,19 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2">
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>62</v>
+      </c>
       <c r="I14" s="29" t="s">
         <v>11</v>
       </c>
@@ -23644,8 +23709,12 @@
       <c r="N14" s="13"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>75</v>
+      </c>
       <c r="I15" s="13" t="s">
         <v>53</v>
       </c>
@@ -23656,8 +23725,12 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>80</v>
+      </c>
       <c r="I16" s="13" t="s">
         <v>34</v>
       </c>
@@ -23668,8 +23741,12 @@
       <c r="N16" s="13"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>88</v>
+      </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13" t="s">
         <v>54</v>
@@ -23680,8 +23757,12 @@
       <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>95</v>
+      </c>
       <c r="I18" s="13"/>
       <c r="J18" s="13" t="s">
         <v>55</v>
@@ -23692,8 +23773,12 @@
       <c r="N18" s="13"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13" t="s">
         <v>56</v>
@@ -26514,12 +26599,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
+      <UserInfo>
+        <DisplayName>Christine Reid</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jim Smith-Wright</DisplayName>
+        <AccountId>57</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26714,28 +26809,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
-      <UserInfo>
-        <DisplayName>Christine Reid</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jim Smith-Wright</DisplayName>
-        <AccountId>57</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="090e8724-afd2-4a00-8d2e-c87448cad135"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26760,18 +26854,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="090e8724-afd2-4a00-8d2e-c87448cad135"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>